<commit_message>
La til resten av eksamensoppgavene
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/skoleeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/skoleeksamen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakon\repositories\met4\tidligere-eksamensoppgaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44F68A0-292E-4A0A-95F5-51BCB82E0646}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7E57DE-631C-4E82-A1CD-2127503A0644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1095" windowWidth="26040" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15240" yWindow="180" windowWidth="15180" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>Semester</t>
   </si>
@@ -72,15 +72,6 @@
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-10-v-fasit.pdf)</t>
   </si>
   <si>
-    <t>Oppgave 1c, 3a-3e</t>
-  </si>
-  <si>
-    <t>Oppgave 1, 2c-2e</t>
-  </si>
-  <si>
-    <t>Oppgave 1c-1e, 3a-3c, 4a-4c</t>
-  </si>
-  <si>
     <t>Ikke lenger pensum per 2021</t>
   </si>
   <si>
@@ -93,9 +84,6 @@
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-10-h-fasit.pdf)</t>
   </si>
   <si>
-    <t>Oppgave 3a-3c</t>
-  </si>
-  <si>
     <t>2011 - Vår</t>
   </si>
   <si>
@@ -105,9 +93,6 @@
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-11-v-fasit.pdf)</t>
   </si>
   <si>
-    <t>Oppgave 1d-1e</t>
-  </si>
-  <si>
     <t>2011 - Høst</t>
   </si>
   <si>
@@ -117,9 +102,6 @@
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-11-h-fasit.pdf)</t>
   </si>
   <si>
-    <t>Oppgave 1a-1f, 3c-3e</t>
-  </si>
-  <si>
     <t>2012 - Vår</t>
   </si>
   <si>
@@ -138,7 +120,184 @@
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-12-h-fasit.pdf)</t>
   </si>
   <si>
-    <t>Oppgave 1a (ANOVA-delen)</t>
+    <t>2013 - Vår</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-13-v.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-13-v-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2013 - Høst</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-13-h.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-13-h-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>1g-1h</t>
+  </si>
+  <si>
+    <t>1a (ANOVA-delen)</t>
+  </si>
+  <si>
+    <t>1a-1f, 3c-3e</t>
+  </si>
+  <si>
+    <t>1d-1e</t>
+  </si>
+  <si>
+    <t>3a-3c</t>
+  </si>
+  <si>
+    <t>1c, 3a-3e</t>
+  </si>
+  <si>
+    <t>1, 2c-2e</t>
+  </si>
+  <si>
+    <t>1c-1e, 3a-3c, 4a-4c</t>
+  </si>
+  <si>
+    <t>2014 - Vår</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-14-v.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-14-v-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>1f-1i</t>
+  </si>
+  <si>
+    <t>2014 - Høst</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-14-h.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-14-h-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2015 - Vår</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-15-v.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-15-v-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2015 - Høst</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-15-h.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-15-h-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2016 - Vår</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-16-v.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-16-v-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2016 - Høst</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-16-h.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-16-h-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2017 - Vår</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-17-v.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-17-v-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>2017 - Høst</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-17-h.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-17-h-fasit.pdf)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1f-1g </t>
+  </si>
+  <si>
+    <t>2018 - Vår</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-18-v.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-18-v-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2018 - Høst</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-18-h.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-18-h-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>1d, 1g</t>
+  </si>
+  <si>
+    <t>2019 - Vår</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-19-v.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-19-v-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2019 - Høst</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-19-h.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-19-h-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2020 - Vår</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-20-v.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-20-v-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2020 - Høst</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-20-h.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-20-h-fasit.pdf)</t>
   </si>
 </sst>
 </file>
@@ -456,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +640,7 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -495,7 +654,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -509,7 +668,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -534,74 +693,271 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>34</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D12" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
La til ikke-relevant oppgave V16 om ANOVA
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/skoleeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/skoleeksamen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakon\repositories\met4\tidligere-eksamensoppgaver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bnarum\misc-repos\met4\tidligere-eksamensoppgaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7E57DE-631C-4E82-A1CD-2127503A0644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2532208-AE49-4624-B9EE-27F6AAD0567F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15240" yWindow="180" windowWidth="15180" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
   <si>
     <t>Semester</t>
   </si>
@@ -617,19 +617,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" customWidth="1"/>
-    <col min="3" max="3" width="66.140625" customWidth="1"/>
-    <col min="4" max="4" width="57.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.26953125" customWidth="1"/>
+    <col min="3" max="3" width="66.1796875" customWidth="1"/>
+    <col min="4" max="4" width="57.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -643,7 +643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -657,7 +657,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -671,7 +671,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -682,7 +682,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -696,7 +696,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -710,7 +710,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -724,7 +724,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -738,7 +738,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -749,7 +749,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -763,7 +763,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -774,7 +774,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -788,7 +788,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -802,7 +802,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -813,7 +813,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -824,7 +824,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -838,7 +838,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -848,8 +848,11 @@
       <c r="C17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -860,7 +863,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -874,7 +877,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -888,7 +891,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -899,7 +902,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -913,7 +916,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>79</v>
       </c>
@@ -927,7 +930,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -938,7 +941,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>85</v>
       </c>
@@ -949,7 +952,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Oppdaterte ikke-relevante oppgaver. Bort med korrelasjonstest.
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/skoleeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/skoleeksamen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bnarum\misc-repos\met4\tidligere-eksamensoppgaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2532208-AE49-4624-B9EE-27F6AAD0567F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1A53B1-12B3-4B92-9CA9-19E046DB951D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
   <si>
     <t>Semester</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-20-h-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2d, 3a-3c</t>
+  </si>
+  <si>
+    <t>1f</t>
   </si>
 </sst>
 </file>
@@ -618,7 +624,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -812,6 +818,9 @@
       <c r="C14" t="s">
         <v>51</v>
       </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -835,7 +844,7 @@
         <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
bort med H13 1n Durbin-test
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/skoleeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/skoleeksamen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bnarum\misc-repos\met4\tidligere-eksamensoppgaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1A53B1-12B3-4B92-9CA9-19E046DB951D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7DA28A-E2B8-44BC-8F3F-F54CAE23B2BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,9 +138,6 @@
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-13-h-fasit.pdf)</t>
   </si>
   <si>
-    <t>1g-1h</t>
-  </si>
-  <si>
     <t>1a (ANOVA-delen)</t>
   </si>
   <si>
@@ -304,6 +301,9 @@
   </si>
   <si>
     <t>1f</t>
+  </si>
+  <si>
+    <t>1g-1h, 1n</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -660,7 +660,7 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -674,7 +674,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -699,7 +699,7 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -713,7 +713,7 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -727,7 +727,7 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -741,7 +741,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -766,7 +766,7 @@
         <v>30</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -791,185 +791,185 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>47</v>
-      </c>
-      <c r="D13" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" t="s">
         <v>49</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>50</v>
       </c>
-      <c r="C14" t="s">
-        <v>51</v>
-      </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
         <v>52</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
         <v>55</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>56</v>
       </c>
-      <c r="C16" t="s">
-        <v>57</v>
-      </c>
       <c r="D16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" t="s">
         <v>58</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>59</v>
       </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
       <c r="D17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
         <v>61</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>62</v>
-      </c>
-      <c r="C18" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
         <v>64</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>65</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>66</v>
-      </c>
-      <c r="D19" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
         <v>68</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>69</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>70</v>
-      </c>
-      <c r="D20" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
         <v>72</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>73</v>
-      </c>
-      <c r="C21" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
         <v>75</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>76</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>77</v>
-      </c>
-      <c r="D22" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
         <v>79</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>80</v>
       </c>
-      <c r="C23" t="s">
-        <v>81</v>
-      </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" t="s">
         <v>82</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>83</v>
-      </c>
-      <c r="C24" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
         <v>85</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>86</v>
-      </c>
-      <c r="C25" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
         <v>88</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>89</v>
-      </c>
-      <c r="C26" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
H09 3c ikke relevant pga ikke-parametrisk test
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/skoleeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/skoleeksamen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hakon\repositories\met4\tidligere-eksamensoppgaver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhhit-my.sharepoint.com/personal/benjamin_narum_nhh_no/Documents/github-repos-bnarum/met4/tidligere-eksamensoppgaver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F55951-4499-4183-8FE5-6833252626E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F2F55951-4499-4183-8FE5-6833252626E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F6F72A2-71B9-451F-BB41-B3F61AD52D34}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
   <si>
     <t>Semester</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-21-h-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>3c</t>
   </si>
 </sst>
 </file>
@@ -642,18 +645,18 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="52.28515625" customWidth="1"/>
-    <col min="3" max="3" width="66.140625" customWidth="1"/>
-    <col min="4" max="4" width="57.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.33203125" customWidth="1"/>
+    <col min="3" max="3" width="66.109375" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -667,7 +670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -681,7 +684,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -695,7 +698,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -705,8 +708,11 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -720,7 +726,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -734,7 +740,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -748,7 +754,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -762,7 +768,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -773,7 +779,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -787,7 +793,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -798,7 +804,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -812,7 +818,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -826,7 +832,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -840,7 +846,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -851,7 +857,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -865,7 +871,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -879,7 +885,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -890,7 +896,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -904,7 +910,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -918,7 +924,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -929,7 +935,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -943,7 +949,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -957,7 +963,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -968,7 +974,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -979,7 +985,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -990,7 +996,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>93</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
Merket som ikke pensum: V14 1e, V15 1c
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/skoleeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/skoleeksamen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhhit-my.sharepoint.com/personal/benjamin_narum_nhh_no/Documents/github-repos-bnarum/met4/tidligere-eksamensoppgaver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F2F55951-4499-4183-8FE5-6833252626E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F6F72A2-71B9-451F-BB41-B3F61AD52D34}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{F2F55951-4499-4183-8FE5-6833252626E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F9A530B-DA3C-427A-916A-8F616F64839E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
   <si>
     <t>Semester</t>
   </si>
@@ -300,9 +300,6 @@
     <t>2d, 3a-3c</t>
   </si>
   <si>
-    <t>1f</t>
-  </si>
-  <si>
     <t>1g-1h, 1n</t>
   </si>
   <si>
@@ -325,6 +322,9 @@
   </si>
   <si>
     <t>3c</t>
+  </si>
+  <si>
+    <t>1e-f</t>
   </si>
 </sst>
 </file>
@@ -645,18 +645,18 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="52.33203125" customWidth="1"/>
-    <col min="3" max="3" width="66.109375" customWidth="1"/>
-    <col min="4" max="4" width="57.6640625" customWidth="1"/>
+    <col min="2" max="2" width="52.36328125" customWidth="1"/>
+    <col min="3" max="3" width="66.08984375" customWidth="1"/>
+    <col min="4" max="4" width="57.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -684,7 +684,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -698,7 +698,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -709,10 +709,10 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -726,7 +726,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -740,7 +740,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -754,7 +754,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -768,7 +768,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -779,7 +779,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -793,7 +793,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -804,7 +804,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -815,10 +815,10 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -832,7 +832,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -843,10 +843,10 @@
         <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -856,8 +856,11 @@
       <c r="C15" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -871,7 +874,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -885,7 +888,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -896,7 +899,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -910,7 +913,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -924,7 +927,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>71</v>
       </c>
@@ -935,7 +938,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -949,7 +952,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -963,7 +966,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>81</v>
       </c>
@@ -974,7 +977,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -985,7 +988,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>87</v>
       </c>
@@ -996,26 +999,26 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" t="s">
         <v>93</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>94</v>
       </c>
-      <c r="C27" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>96</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>97</v>
-      </c>
-      <c r="C28" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
H17 1h er ikke pensum
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/skoleeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/skoleeksamen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nhhit-my.sharepoint.com/personal/benjamin_narum_nhh_no/Documents/github-repos-bnarum/met4/tidligere-eksamensoppgaver/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bnarum\OneDrive - Norges Handelshøyskole\github-repos-bnarum\met4\tidligere-eksamensoppgaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{F2F55951-4499-4183-8FE5-6833252626E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9F9A530B-DA3C-427A-916A-8F616F64839E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A240F969-A4DA-491F-9956-A0659B97921C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="3540" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -237,9 +237,6 @@
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-17-h-fasit.pdf)</t>
   </si>
   <si>
-    <t xml:space="preserve">1f-1g </t>
-  </si>
-  <si>
     <t>2018 - Vår</t>
   </si>
   <si>
@@ -325,6 +322,9 @@
   </si>
   <si>
     <t>1e-f</t>
+  </si>
+  <si>
+    <t>1f-1h</t>
   </si>
 </sst>
 </file>
@@ -644,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -709,7 +709,7 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -815,7 +815,7 @@
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -871,7 +871,7 @@
         <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
@@ -924,43 +924,43 @@
         <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
         <v>71</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>72</v>
-      </c>
-      <c r="C21" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" t="s">
         <v>74</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>75</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>76</v>
-      </c>
-      <c r="D22" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" t="s">
         <v>78</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>79</v>
-      </c>
-      <c r="C23" t="s">
-        <v>80</v>
       </c>
       <c r="D23" t="s">
         <v>66</v>
@@ -968,57 +968,57 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24" t="s">
         <v>81</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>82</v>
-      </c>
-      <c r="C24" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
         <v>84</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>85</v>
-      </c>
-      <c r="C25" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" t="s">
         <v>87</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>88</v>
-      </c>
-      <c r="C26" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
         <v>92</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>93</v>
-      </c>
-      <c r="C27" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
         <v>95</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>96</v>
-      </c>
-      <c r="C28" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
la til skoleeksamen V22
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/skoleeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/skoleeksamen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bnarum\OneDrive - Norges Handelshøyskole\github-repos-bnarum\met4\tidligere-eksamensoppgaver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s12203\repos\met4\tidligere-eksamensoppgaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A240F969-A4DA-491F-9956-A0659B97921C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAA9A7F-EEFB-45C6-ACA4-FEE2504CA4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="3540" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-195" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="103">
   <si>
     <t>Semester</t>
   </si>
@@ -325,6 +325,15 @@
   </si>
   <si>
     <t>1f-1h</t>
+  </si>
+  <si>
+    <t>2022 - Vår</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-22-v.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-22-v-fasit.pdf)</t>
   </si>
 </sst>
 </file>
@@ -642,21 +651,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="52.36328125" customWidth="1"/>
-    <col min="3" max="3" width="66.08984375" customWidth="1"/>
-    <col min="4" max="4" width="57.6328125" customWidth="1"/>
+    <col min="2" max="2" width="52.42578125" customWidth="1"/>
+    <col min="3" max="3" width="66.140625" customWidth="1"/>
+    <col min="4" max="4" width="57.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -670,7 +679,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -684,7 +693,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -698,7 +707,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -712,7 +721,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -726,7 +735,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -740,7 +749,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -754,7 +763,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -768,7 +777,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -779,7 +788,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -793,7 +802,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -804,7 +813,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -818,7 +827,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -832,7 +841,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -846,7 +855,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -860,7 +869,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -874,7 +883,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -888,7 +897,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -899,7 +908,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -913,7 +922,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>67</v>
       </c>
@@ -927,7 +936,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -938,7 +947,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>73</v>
       </c>
@@ -952,7 +961,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -966,7 +975,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -977,7 +986,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -988,7 +997,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>86</v>
       </c>
@@ -999,7 +1008,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>91</v>
       </c>
@@ -1010,7 +1019,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -1019,6 +1028,17 @@
       </c>
       <c r="C28" t="s">
         <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>100</v>
+      </c>
+      <c r="B29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
oppdaterte fpp til fpp2 i tidsrekkemodulen og la til eksamen h24
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/skoleeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/skoleeksamen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\met4\tidligere-eksamensoppgaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5186692D-97A4-462F-9E7D-75B8074A22B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86848B98-C3E7-4F84-B605-FB3BCB11F8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="25996" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Semester</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-24-v-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2024 - Høst</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-24-h.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-24-h-fasit.pdf)</t>
   </si>
 </sst>
 </file>
@@ -498,21 +507,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="52.453125" customWidth="1"/>
-    <col min="3" max="3" width="66.08984375" customWidth="1"/>
-    <col min="4" max="4" width="57.54296875" customWidth="1"/>
+    <col min="2" max="2" width="52.46484375" customWidth="1"/>
+    <col min="3" max="3" width="66.06640625" customWidth="1"/>
+    <col min="4" max="4" width="57.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -526,7 +535,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -540,7 +549,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -554,7 +563,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -565,7 +574,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -579,7 +588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -593,7 +602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -604,7 +613,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -615,7 +624,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -626,7 +635,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -637,7 +646,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -648,7 +657,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -659,7 +668,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -670,7 +679,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -681,7 +690,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -692,7 +701,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -701,6 +710,17 @@
       </c>
       <c r="C16" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
oppdaterte fremside til h25 og lagt til vårens eksamensoppgave
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/skoleeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/skoleeksamen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\met4\tidligere-eksamensoppgaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86848B98-C3E7-4F84-B605-FB3BCB11F8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8604D75A-D235-4A4E-9D74-31946AB5F991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="25996" windowHeight="10276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Semester</t>
   </si>
@@ -190,6 +190,15 @@
   </si>
   <si>
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-24-h-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>2025 - Vår</t>
+  </si>
+  <si>
+    <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-25-v.pdf)</t>
+  </si>
+  <si>
+    <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-25-v-fasit.pdf)</t>
   </si>
 </sst>
 </file>
@@ -507,21 +516,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="52.46484375" customWidth="1"/>
-    <col min="3" max="3" width="66.06640625" customWidth="1"/>
-    <col min="4" max="4" width="57.53125" customWidth="1"/>
+    <col min="2" max="2" width="52.453125" customWidth="1"/>
+    <col min="3" max="3" width="66.08984375" customWidth="1"/>
+    <col min="4" max="4" width="57.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,7 +544,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -549,7 +558,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -563,7 +572,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -574,7 +583,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -588,7 +597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -602,7 +611,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -613,7 +622,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -624,7 +633,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -635,7 +644,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -646,7 +655,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -657,7 +666,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -668,7 +677,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -679,7 +688,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -690,7 +699,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -701,7 +710,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>49</v>
       </c>
@@ -712,7 +721,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -721,6 +730,17 @@
       </c>
       <c r="C17" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
småplukk og v25 eksamen lagt til på ny
</commit_message>
<xml_diff>
--- a/tidligere-eksamensoppgaver/skoleeksamen.xlsx
+++ b/tidligere-eksamensoppgaver/skoleeksamen.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\met4\tidligere-eksamensoppgaver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8604D75A-D235-4A4E-9D74-31946AB5F991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{755E829F-F33E-46EA-9954-DA95EB63E674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Semester</t>
   </si>
@@ -153,9 +153,6 @@
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-22-h-fasit.pdf)</t>
   </si>
   <si>
-    <t>Ikke lenger pensum per 2023</t>
-  </si>
-  <si>
     <t>[Oppgaveformulering](tidligere-eksamensoppgaver/skole-23-v.pdf)</t>
   </si>
   <si>
@@ -199,6 +196,15 @@
   </si>
   <si>
     <t>[Løsningsforslag](tidligere-eksamensoppgaver/skole-25-v-fasit.pdf)</t>
+  </si>
+  <si>
+    <t>Ikke lenger pensum per 2025</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>[Materiale](tidligere-eksamensoppgaver/skole-25-v-ekstra.zip)</t>
   </si>
 </sst>
 </file>
@@ -516,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -528,9 +534,11 @@
     <col min="2" max="2" width="52.453125" customWidth="1"/>
     <col min="3" max="3" width="66.08984375" customWidth="1"/>
     <col min="4" max="4" width="57.54296875" customWidth="1"/>
+    <col min="5" max="5" width="56.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -541,10 +549,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -558,7 +569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -572,7 +583,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -583,7 +594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -597,7 +608,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -611,7 +622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -622,7 +633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -633,7 +644,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -644,7 +655,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -655,7 +666,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -666,7 +677,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -677,7 +688,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -688,59 +699,62 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="B14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>46</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>47</v>
       </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>49</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>50</v>
       </c>
-      <c r="C16" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>52</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>53</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>55</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>56</v>
       </c>
-      <c r="C18" t="s">
-        <v>57</v>
+      <c r="E18" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>